<commit_message>
Modifying excel biostudies file
</commit_message>
<xml_diff>
--- a/data/biostudies/hepatic/Valproic_Acid_Hepatic_Biostudies.xlsx
+++ b/data/biostudies/hepatic/Valproic_Acid_Hepatic_Biostudies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="175">
   <si>
     <t>Study</t>
   </si>
@@ -530,6 +530,15 @@
   </si>
   <si>
     <t>0897</t>
+  </si>
+  <si>
+    <t>0982</t>
+  </si>
+  <si>
+    <t>0983</t>
+  </si>
+  <si>
+    <t>0984</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1098,7 @@
     <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1154,7 +1163,6 @@
     <xf numFmtId="14" fontId="7" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1167,7 +1175,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1526,8 +1533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1781,7 +1788,7 @@
       <c r="A22" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="31" t="s">
         <v>73</v>
       </c>
       <c r="C22" s="10"/>
@@ -1825,7 +1832,7 @@
       <c r="A26" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="34" t="s">
         <v>72</v>
       </c>
       <c r="G26" s="11"/>
@@ -1855,7 +1862,7 @@
       <c r="A29" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="35" t="s">
         <v>169</v>
       </c>
       <c r="C29" s="29">
@@ -1864,7 +1871,7 @@
       <c r="D29" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E29" s="34" t="s">
+      <c r="E29" s="33" t="s">
         <v>70</v>
       </c>
       <c r="F29" s="22" t="s">
@@ -1875,18 +1882,18 @@
       <c r="A30" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B30" s="38" t="str">
+      <c r="B30" s="36" t="str">
         <f>B29</f>
         <v>0895</v>
       </c>
-      <c r="C30" s="33">
+      <c r="C30" s="32">
         <f>C29</f>
         <v>42822</v>
       </c>
       <c r="D30" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E30" s="34" t="s">
+      <c r="E30" s="33" t="s">
         <v>70</v>
       </c>
       <c r="F30" s="22" t="s">
@@ -1897,17 +1904,17 @@
       <c r="A31" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="C31" s="33">
+      <c r="C31" s="32">
         <f t="shared" ref="C31:C46" si="0">C30</f>
         <v>42822</v>
       </c>
       <c r="D31" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="33" t="s">
         <v>70</v>
       </c>
       <c r="F31" s="22" t="s">
@@ -1918,17 +1925,17 @@
       <c r="A32" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="C32" s="33">
+      <c r="C32" s="32">
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
       <c r="D32" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="33" t="s">
         <v>70</v>
       </c>
       <c r="F32" s="22" t="s">
@@ -1939,17 +1946,17 @@
       <c r="A33" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="C33" s="33">
+      <c r="C33" s="32">
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E33" s="34" t="s">
+      <c r="E33" s="33" t="s">
         <v>70</v>
       </c>
       <c r="F33" s="22" t="s">
@@ -1960,17 +1967,17 @@
       <c r="A34" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="C34" s="33">
+      <c r="C34" s="32">
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
       <c r="D34" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="E34" s="33" t="s">
         <v>70</v>
       </c>
       <c r="F34" s="22" t="s">
@@ -1981,10 +1988,10 @@
       <c r="A35" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="30">
+      <c r="B35" s="36">
         <v>919</v>
       </c>
-      <c r="C35" s="33">
+      <c r="C35" s="32">
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
@@ -2002,11 +2009,11 @@
       <c r="A36" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B36" s="30">
+      <c r="B36" s="36">
         <f>B35</f>
         <v>919</v>
       </c>
-      <c r="C36" s="33">
+      <c r="C36" s="32">
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
@@ -2024,11 +2031,11 @@
       <c r="A37" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="30">
+      <c r="B37" s="36">
         <f>B35+1</f>
         <v>920</v>
       </c>
-      <c r="C37" s="33">
+      <c r="C37" s="32">
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
@@ -2046,11 +2053,11 @@
       <c r="A38" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="30">
+      <c r="B38" s="36">
         <f>B37</f>
         <v>920</v>
       </c>
-      <c r="C38" s="33">
+      <c r="C38" s="32">
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
@@ -2068,11 +2075,11 @@
       <c r="A39" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B39" s="30">
+      <c r="B39" s="36">
         <f>B37+1</f>
         <v>921</v>
       </c>
-      <c r="C39" s="33">
+      <c r="C39" s="32">
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
@@ -2090,11 +2097,11 @@
       <c r="A40" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B40" s="30">
+      <c r="B40" s="36">
         <f>B39</f>
         <v>921</v>
       </c>
-      <c r="C40" s="33">
+      <c r="C40" s="32">
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
@@ -2112,11 +2119,11 @@
       <c r="A41" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B41" s="30">
+      <c r="B41" s="36">
         <f>B39+1</f>
         <v>922</v>
       </c>
-      <c r="C41" s="33">
+      <c r="C41" s="32">
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
@@ -2134,11 +2141,11 @@
       <c r="A42" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B42" s="30">
+      <c r="B42" s="36">
         <f>B41</f>
         <v>922</v>
       </c>
-      <c r="C42" s="33">
+      <c r="C42" s="32">
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
@@ -2156,11 +2163,11 @@
       <c r="A43" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="B43" s="30">
+      <c r="B43" s="36">
         <f>B41+1</f>
         <v>923</v>
       </c>
-      <c r="C43" s="33">
+      <c r="C43" s="32">
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
@@ -2178,11 +2185,11 @@
       <c r="A44" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="30">
+      <c r="B44" s="36">
         <f>B43</f>
         <v>923</v>
       </c>
-      <c r="C44" s="33">
+      <c r="C44" s="32">
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
@@ -2200,11 +2207,11 @@
       <c r="A45" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="30">
+      <c r="B45" s="36">
         <f>B43+1</f>
         <v>924</v>
       </c>
-      <c r="C45" s="33">
+      <c r="C45" s="32">
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
@@ -2222,11 +2229,11 @@
       <c r="A46" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="B46" s="30">
+      <c r="B46" s="36">
         <f>B45</f>
         <v>924</v>
       </c>
-      <c r="C46" s="33">
+      <c r="C46" s="32">
         <f t="shared" si="0"/>
         <v>42822</v>
       </c>
@@ -2244,7 +2251,7 @@
       <c r="A47" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="B47" s="30">
+      <c r="B47" s="36">
         <f>B45+1</f>
         <v>925</v>
       </c>
@@ -2265,7 +2272,7 @@
       <c r="A48" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="30">
+      <c r="B48" s="36">
         <f>B47</f>
         <v>925</v>
       </c>
@@ -2287,7 +2294,7 @@
       <c r="A49" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="30">
+      <c r="B49" s="36">
         <f>B47+1</f>
         <v>926</v>
       </c>
@@ -2309,7 +2316,7 @@
       <c r="A50" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B50" s="30">
+      <c r="B50" s="36">
         <f>B49</f>
         <v>926</v>
       </c>
@@ -2331,7 +2338,7 @@
       <c r="A51" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="30">
+      <c r="B51" s="36">
         <f>B49+1</f>
         <v>927</v>
       </c>
@@ -2353,7 +2360,7 @@
       <c r="A52" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="30">
+      <c r="B52" s="36">
         <f>B51</f>
         <v>927</v>
       </c>
@@ -2375,7 +2382,7 @@
       <c r="A53" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="B53" s="30">
+      <c r="B53" s="36">
         <f>B51+1</f>
         <v>928</v>
       </c>
@@ -2396,7 +2403,7 @@
       <c r="A54" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="B54" s="30">
+      <c r="B54" s="36">
         <f>B53</f>
         <v>928</v>
       </c>
@@ -2418,7 +2425,7 @@
       <c r="A55" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="B55" s="30">
+      <c r="B55" s="36">
         <f>B53+1</f>
         <v>929</v>
       </c>
@@ -2440,7 +2447,7 @@
       <c r="A56" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="B56" s="30">
+      <c r="B56" s="36">
         <f>B55</f>
         <v>929</v>
       </c>
@@ -2462,7 +2469,7 @@
       <c r="A57" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="30">
+      <c r="B57" s="36">
         <f>B55+1</f>
         <v>930</v>
       </c>
@@ -2484,7 +2491,7 @@
       <c r="A58" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="B58" s="30">
+      <c r="B58" s="36">
         <f>B57</f>
         <v>930</v>
       </c>
@@ -2506,7 +2513,7 @@
       <c r="A59" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="B59" s="30">
+      <c r="B59" s="36">
         <f>B57+1</f>
         <v>931</v>
       </c>
@@ -2527,7 +2534,7 @@
       <c r="A60" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="B60" s="30">
+      <c r="B60" s="36">
         <f>B59</f>
         <v>931</v>
       </c>
@@ -2549,7 +2556,7 @@
       <c r="A61" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B61" s="30">
+      <c r="B61" s="36">
         <f>B59+1</f>
         <v>932</v>
       </c>
@@ -2571,7 +2578,7 @@
       <c r="A62" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B62" s="30">
+      <c r="B62" s="36">
         <f>B61</f>
         <v>932</v>
       </c>
@@ -2593,7 +2600,7 @@
       <c r="A63" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="B63" s="30">
+      <c r="B63" s="36">
         <f>B61+1</f>
         <v>933</v>
       </c>
@@ -2615,7 +2622,7 @@
       <c r="A64" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="B64" s="30">
+      <c r="B64" s="36">
         <f>B63</f>
         <v>933</v>
       </c>
@@ -2637,7 +2644,7 @@
       <c r="A65" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B65" s="30">
+      <c r="B65" s="36">
         <f>B63+1</f>
         <v>934</v>
       </c>
@@ -2658,7 +2665,7 @@
       <c r="A66" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="B66" s="30">
+      <c r="B66" s="36">
         <f>B65</f>
         <v>934</v>
       </c>
@@ -2680,7 +2687,7 @@
       <c r="A67" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="B67" s="30">
+      <c r="B67" s="36">
         <f>B65+1</f>
         <v>935</v>
       </c>
@@ -2702,7 +2709,7 @@
       <c r="A68" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="B68" s="30">
+      <c r="B68" s="36">
         <f>B67</f>
         <v>935</v>
       </c>
@@ -2724,7 +2731,7 @@
       <c r="A69" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="B69" s="30">
+      <c r="B69" s="36">
         <f>B67+1</f>
         <v>936</v>
       </c>
@@ -2746,7 +2753,7 @@
       <c r="A70" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="B70" s="30">
+      <c r="B70" s="36">
         <f>B69</f>
         <v>936</v>
       </c>
@@ -2768,7 +2775,7 @@
       <c r="A71" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="B71" s="30">
+      <c r="B71" s="36">
         <f>B69+1</f>
         <v>937</v>
       </c>
@@ -2789,7 +2796,7 @@
       <c r="A72" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B72" s="30">
+      <c r="B72" s="36">
         <f>B71</f>
         <v>937</v>
       </c>
@@ -2811,7 +2818,7 @@
       <c r="A73" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="B73" s="30">
+      <c r="B73" s="36">
         <f>B71+1</f>
         <v>938</v>
       </c>
@@ -2833,7 +2840,7 @@
       <c r="A74" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="B74" s="30">
+      <c r="B74" s="36">
         <f>B73</f>
         <v>938</v>
       </c>
@@ -2855,7 +2862,7 @@
       <c r="A75" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="B75" s="30">
+      <c r="B75" s="36">
         <f>B73+1</f>
         <v>939</v>
       </c>
@@ -2877,7 +2884,7 @@
       <c r="A76" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B76" s="30">
+      <c r="B76" s="36">
         <f>B75</f>
         <v>939</v>
       </c>
@@ -2899,8 +2906,8 @@
       <c r="A77" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B77" s="35">
-        <v>982</v>
+      <c r="B77" s="35" t="s">
+        <v>172</v>
       </c>
       <c r="C77" s="29">
         <v>42899</v>
@@ -2908,7 +2915,7 @@
       <c r="D77" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E77" s="34" t="s">
+      <c r="E77" s="33" t="s">
         <v>70</v>
       </c>
       <c r="F77" s="22" t="s">
@@ -2919,18 +2926,17 @@
       <c r="A78" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B78" s="30">
-        <f>B77</f>
-        <v>982</v>
-      </c>
-      <c r="C78" s="33">
+      <c r="B78" s="36" t="s">
+        <v>172</v>
+      </c>
+      <c r="C78" s="32">
         <f>C77</f>
         <v>42899</v>
       </c>
       <c r="D78" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E78" s="34" t="s">
+      <c r="E78" s="33" t="s">
         <v>70</v>
       </c>
       <c r="F78" s="22" t="s">
@@ -2941,18 +2947,17 @@
       <c r="A79" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="B79" s="30">
-        <f>B77+1</f>
-        <v>983</v>
-      </c>
-      <c r="C79" s="33">
+      <c r="B79" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C79" s="32">
         <f t="shared" ref="C79:C94" si="1">C78</f>
         <v>42899</v>
       </c>
       <c r="D79" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E79" s="34" t="s">
+      <c r="E79" s="33" t="s">
         <v>70</v>
       </c>
       <c r="F79" s="22" t="s">
@@ -2963,18 +2968,17 @@
       <c r="A80" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="B80" s="30">
-        <f>B79</f>
-        <v>983</v>
-      </c>
-      <c r="C80" s="33">
+      <c r="B80" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="C80" s="32">
         <f t="shared" si="1"/>
         <v>42899</v>
       </c>
       <c r="D80" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E80" s="34" t="s">
+      <c r="E80" s="33" t="s">
         <v>70</v>
       </c>
       <c r="F80" s="22" t="s">
@@ -2985,18 +2989,17 @@
       <c r="A81" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="B81" s="30">
-        <f>B79+1</f>
-        <v>984</v>
-      </c>
-      <c r="C81" s="33">
+      <c r="B81" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="C81" s="32">
         <f t="shared" si="1"/>
         <v>42899</v>
       </c>
       <c r="D81" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E81" s="34" t="s">
+      <c r="E81" s="33" t="s">
         <v>70</v>
       </c>
       <c r="F81" s="22" t="s">
@@ -3007,18 +3010,17 @@
       <c r="A82" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="B82" s="30">
-        <f>B81</f>
-        <v>984</v>
-      </c>
-      <c r="C82" s="33">
+      <c r="B82" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="C82" s="32">
         <f t="shared" si="1"/>
         <v>42899</v>
       </c>
       <c r="D82" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E82" s="34" t="s">
+      <c r="E82" s="33" t="s">
         <v>70</v>
       </c>
       <c r="F82" s="22" t="s">
@@ -3029,10 +3031,10 @@
       <c r="A83" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="B83" s="30">
+      <c r="B83" s="36">
         <v>1003</v>
       </c>
-      <c r="C83" s="33">
+      <c r="C83" s="32">
         <f t="shared" si="1"/>
         <v>42899</v>
       </c>
@@ -3050,11 +3052,11 @@
       <c r="A84" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="B84" s="30">
+      <c r="B84" s="36">
         <f>B83</f>
         <v>1003</v>
       </c>
-      <c r="C84" s="33">
+      <c r="C84" s="32">
         <f t="shared" si="1"/>
         <v>42899</v>
       </c>
@@ -3072,11 +3074,11 @@
       <c r="A85" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="B85" s="30">
+      <c r="B85" s="36">
         <f>B83+1</f>
         <v>1004</v>
       </c>
-      <c r="C85" s="33">
+      <c r="C85" s="32">
         <f t="shared" si="1"/>
         <v>42899</v>
       </c>
@@ -3094,11 +3096,11 @@
       <c r="A86" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B86" s="30">
+      <c r="B86" s="36">
         <f>B85</f>
         <v>1004</v>
       </c>
-      <c r="C86" s="33">
+      <c r="C86" s="32">
         <f t="shared" si="1"/>
         <v>42899</v>
       </c>
@@ -3116,11 +3118,11 @@
       <c r="A87" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="B87" s="30">
+      <c r="B87" s="36">
         <f>B85+1</f>
         <v>1005</v>
       </c>
-      <c r="C87" s="33">
+      <c r="C87" s="32">
         <f t="shared" si="1"/>
         <v>42899</v>
       </c>
@@ -3138,11 +3140,11 @@
       <c r="A88" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="B88" s="30">
+      <c r="B88" s="36">
         <f>B87</f>
         <v>1005</v>
       </c>
-      <c r="C88" s="33">
+      <c r="C88" s="32">
         <f t="shared" si="1"/>
         <v>42899</v>
       </c>
@@ -3160,11 +3162,11 @@
       <c r="A89" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="B89" s="30">
+      <c r="B89" s="36">
         <f>B87+1</f>
         <v>1006</v>
       </c>
-      <c r="C89" s="33">
+      <c r="C89" s="32">
         <f t="shared" si="1"/>
         <v>42899</v>
       </c>
@@ -3182,11 +3184,11 @@
       <c r="A90" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="B90" s="30">
+      <c r="B90" s="36">
         <f>B89</f>
         <v>1006</v>
       </c>
-      <c r="C90" s="33">
+      <c r="C90" s="32">
         <f t="shared" si="1"/>
         <v>42899</v>
       </c>
@@ -3204,11 +3206,11 @@
       <c r="A91" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="B91" s="30">
+      <c r="B91" s="36">
         <f>B89+1</f>
         <v>1007</v>
       </c>
-      <c r="C91" s="33">
+      <c r="C91" s="32">
         <f t="shared" si="1"/>
         <v>42899</v>
       </c>
@@ -3226,11 +3228,11 @@
       <c r="A92" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="B92" s="30">
+      <c r="B92" s="36">
         <f>B91</f>
         <v>1007</v>
       </c>
-      <c r="C92" s="33">
+      <c r="C92" s="32">
         <f t="shared" si="1"/>
         <v>42899</v>
       </c>
@@ -3248,11 +3250,11 @@
       <c r="A93" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="B93" s="30">
+      <c r="B93" s="36">
         <f>B91+1</f>
         <v>1008</v>
       </c>
-      <c r="C93" s="33">
+      <c r="C93" s="32">
         <f t="shared" si="1"/>
         <v>42899</v>
       </c>
@@ -3270,11 +3272,11 @@
       <c r="A94" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="B94" s="30">
+      <c r="B94" s="36">
         <f>B93</f>
         <v>1008</v>
       </c>
-      <c r="C94" s="33">
+      <c r="C94" s="32">
         <f t="shared" si="1"/>
         <v>42899</v>
       </c>
@@ -3292,7 +3294,7 @@
       <c r="A95" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B95" s="30">
+      <c r="B95" s="36">
         <f>B93+1</f>
         <v>1009</v>
       </c>
@@ -3313,7 +3315,7 @@
       <c r="A96" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="B96" s="30">
+      <c r="B96" s="36">
         <f>B95</f>
         <v>1009</v>
       </c>
@@ -3335,7 +3337,7 @@
       <c r="A97" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="B97" s="30">
+      <c r="B97" s="36">
         <f>B95+1</f>
         <v>1010</v>
       </c>
@@ -3357,7 +3359,7 @@
       <c r="A98" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="B98" s="30">
+      <c r="B98" s="36">
         <f>B97</f>
         <v>1010</v>
       </c>
@@ -3379,7 +3381,7 @@
       <c r="A99" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="B99" s="30">
+      <c r="B99" s="36">
         <f>B97+1</f>
         <v>1011</v>
       </c>
@@ -3401,7 +3403,7 @@
       <c r="A100" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="B100" s="30">
+      <c r="B100" s="36">
         <f>B99</f>
         <v>1011</v>
       </c>
@@ -3423,7 +3425,7 @@
       <c r="A101" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="B101" s="30">
+      <c r="B101" s="36">
         <f>B99+1</f>
         <v>1012</v>
       </c>
@@ -3444,7 +3446,7 @@
       <c r="A102" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="B102" s="30">
+      <c r="B102" s="36">
         <f>B101</f>
         <v>1012</v>
       </c>
@@ -3466,7 +3468,7 @@
       <c r="A103" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="B103" s="30">
+      <c r="B103" s="36">
         <f>B101+1</f>
         <v>1013</v>
       </c>
@@ -3488,7 +3490,7 @@
       <c r="A104" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="B104" s="30">
+      <c r="B104" s="36">
         <f>B103</f>
         <v>1013</v>
       </c>
@@ -3510,7 +3512,7 @@
       <c r="A105" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="B105" s="30">
+      <c r="B105" s="36">
         <f>B103+1</f>
         <v>1014</v>
       </c>
@@ -3532,7 +3534,7 @@
       <c r="A106" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="B106" s="30">
+      <c r="B106" s="36">
         <f>B105</f>
         <v>1014</v>
       </c>
@@ -3554,7 +3556,7 @@
       <c r="A107" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="B107" s="30">
+      <c r="B107" s="36">
         <f>B105+1</f>
         <v>1015</v>
       </c>
@@ -3575,7 +3577,7 @@
       <c r="A108" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="B108" s="30">
+      <c r="B108" s="36">
         <f>B107</f>
         <v>1015</v>
       </c>
@@ -3597,7 +3599,7 @@
       <c r="A109" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="B109" s="30">
+      <c r="B109" s="36">
         <f>B107+1</f>
         <v>1016</v>
       </c>
@@ -3619,7 +3621,7 @@
       <c r="A110" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="B110" s="30">
+      <c r="B110" s="36">
         <f>B109</f>
         <v>1016</v>
       </c>
@@ -3641,7 +3643,7 @@
       <c r="A111" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="B111" s="30">
+      <c r="B111" s="36">
         <f>B109+1</f>
         <v>1017</v>
       </c>
@@ -3663,7 +3665,7 @@
       <c r="A112" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="B112" s="30">
+      <c r="B112" s="36">
         <f>B111</f>
         <v>1017</v>
       </c>
@@ -3685,7 +3687,7 @@
       <c r="A113" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="B113" s="30">
+      <c r="B113" s="36">
         <f>B111+1</f>
         <v>1018</v>
       </c>
@@ -3706,7 +3708,7 @@
       <c r="A114" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="B114" s="30">
+      <c r="B114" s="36">
         <f>B113</f>
         <v>1018</v>
       </c>
@@ -3728,7 +3730,7 @@
       <c r="A115" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="B115" s="30">
+      <c r="B115" s="36">
         <f>B113+1</f>
         <v>1019</v>
       </c>
@@ -3750,7 +3752,7 @@
       <c r="A116" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="B116" s="30">
+      <c r="B116" s="36">
         <f>B115</f>
         <v>1019</v>
       </c>
@@ -3772,7 +3774,7 @@
       <c r="A117" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="B117" s="30">
+      <c r="B117" s="36">
         <f>B115+1</f>
         <v>1020</v>
       </c>
@@ -3794,7 +3796,7 @@
       <c r="A118" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="B118" s="30">
+      <c r="B118" s="36">
         <f>B117</f>
         <v>1020</v>
       </c>
@@ -3813,7 +3815,7 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A119" s="31" t="s">
+      <c r="A119" s="30" t="s">
         <v>78</v>
       </c>
       <c r="B119" s="26"/>

</xml_diff>